<commit_message>
Amélioration de la documentation
</commit_message>
<xml_diff>
--- a/Page_Web_ICT120/Documentation/Use case.xlsx
+++ b/Page_Web_ICT120/Documentation/Use case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CPNV-----------------------------------------------------------------------\ICT-120\Page_Web_ICT120\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0469BF19-2F61-4DC3-8D3C-E82261AC636A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC2B77B-2F6A-4AAB-A670-B8BEB6055F00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="78">
   <si>
     <t>Identifiant</t>
   </si>
@@ -72,12 +72,6 @@
     <t>presse sur "supprimer"</t>
   </si>
   <si>
-    <t>selectionner une activité</t>
-  </si>
-  <si>
-    <t>mieu la comprendre</t>
-  </si>
-  <si>
     <t>presse sur la barre pour inscrire son email</t>
   </si>
   <si>
@@ -123,24 +117,9 @@
     <t>rafraîchi la page</t>
   </si>
   <si>
-    <t>presse sur le Menu</t>
-  </si>
-  <si>
     <t>Use case Page d'activité avec login</t>
   </si>
   <si>
-    <t xml:space="preserve">ouvre un onglet a gauche de la page avec inscrit dedans:Déconnection et Intranet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">si il presse sur Déconnection </t>
-  </si>
-  <si>
-    <t>arenvoie sur la page d'activité sans être login(ou sans login)</t>
-  </si>
-  <si>
-    <t>sil il presse sur Intranet</t>
-  </si>
-  <si>
     <t>renvoie sur la page Intranet</t>
   </si>
   <si>
@@ -192,27 +171,12 @@
     <t>presse sur Lieu et heure de rdv</t>
   </si>
   <si>
-    <t xml:space="preserve">ouvre un onglet a gauche de la page avec inscrit dedans: Login , Register et Intranet </t>
-  </si>
-  <si>
-    <t>si il presse sur Login</t>
-  </si>
-  <si>
     <t>affiche la page pour ce login</t>
   </si>
   <si>
-    <t xml:space="preserve">si il presse sur Register </t>
-  </si>
-  <si>
     <t>affiche la page pour ce créer un compte (page Register)</t>
   </si>
   <si>
-    <t xml:space="preserve">si presse ssur la croix en-haut a droite </t>
-  </si>
-  <si>
-    <t>ferme l'onglet menu</t>
-  </si>
-  <si>
     <t>Use case page Register</t>
   </si>
   <si>
@@ -240,23 +204,68 @@
     <t>affiche une alert indiquant que soit l'email ou soit le mot de passe est incorect</t>
   </si>
   <si>
-    <t>si il presse sur Menu blanc</t>
-  </si>
-  <si>
     <t>la couleur de fond du bando, fil d'arianne et titre activité passe en blanche</t>
   </si>
   <si>
-    <t>si il presse sur Menu turquoise</t>
-  </si>
-  <si>
     <t>la couleur de fond du bando, fil d'arianne et titre activité passe en turquoise</t>
+  </si>
+  <si>
+    <t>presse Login</t>
+  </si>
+  <si>
+    <t>presse sur Menu blanc</t>
+  </si>
+  <si>
+    <t>presse sur Menu turquoise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presse sur Register </t>
+  </si>
+  <si>
+    <t>presse sur Intranet</t>
+  </si>
+  <si>
+    <t>presse sur modifier</t>
+  </si>
+  <si>
+    <t>cache le bouton Modifier et met a sa place le bouton Enrgistrer</t>
+  </si>
+  <si>
+    <t>sil il y au minimum une ligne ajouté</t>
+  </si>
+  <si>
+    <t>cache le bouton Modifier et met a sa place le bouton Enrgistrer chaque champ peuvent être modifier uniquement en texte</t>
+  </si>
+  <si>
+    <t>presse sur Enrgistrer</t>
+  </si>
+  <si>
+    <t>réaffiche tout les champ qui on été modifier avec leur modification</t>
+  </si>
+  <si>
+    <t>voir la page des activités</t>
+  </si>
+  <si>
+    <t>pouvoir en ajouter/supprimer/modifier une ou plusieurs</t>
+  </si>
+  <si>
+    <t>presse sur Deconnexion</t>
+  </si>
+  <si>
+    <t>affiche la page d'activités sans être connecté (page activité sans login)</t>
+  </si>
+  <si>
+    <t>presse sur supprimer</t>
+  </si>
+  <si>
+    <t>si il n'y a aucune ligne ajouté</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,13 +275,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -306,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -525,17 +527,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -545,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -610,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -625,14 +616,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:H106"/>
+  <dimension ref="B5:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,10 +932,10 @@
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+        <v>30</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -972,16 +960,16 @@
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -1016,7 +1004,7 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1025,393 +1013,411 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="28" t="s">
+        <v>62</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
-      <c r="C19" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-      <c r="C21" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
-      <c r="C22" s="15" t="s">
+    <row r="23" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="15"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>77</v>
+      </c>
       <c r="D24" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="19"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="D25" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="16" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="16" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="20" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="20" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="20" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>0</v>
+      <c r="B39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="D40" s="3"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>15</v>
+    <row r="41" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>16</v>
-      </c>
+    <row r="42" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>9</v>
+      <c r="B45" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="13" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B47" s="28" t="s">
+        <v>62</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="16" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B48" s="24" t="s">
-        <v>32</v>
+      <c r="B48" s="28" t="s">
+        <v>63</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="28"/>
-      <c r="C49" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="B49" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="15"/>
       <c r="D49" s="16" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="28"/>
-      <c r="C50" s="15" t="s">
-        <v>56</v>
-      </c>
+      <c r="B50" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="15"/>
       <c r="D50" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="28"/>
-      <c r="C51" s="15" t="s">
-        <v>71</v>
-      </c>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B51" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="15"/>
       <c r="D51" s="16" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B52" s="28"/>
-      <c r="C52" s="15" t="s">
-        <v>73</v>
-      </c>
+      <c r="B52" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="19"/>
       <c r="D52" s="16" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="28"/>
-      <c r="C53" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="B53" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="15"/>
       <c r="D53" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="25"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B54" s="24" t="s">
+        <v>66</v>
+      </c>
       <c r="C54" s="15" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B55" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C55" s="15"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B55" s="25"/>
+      <c r="C55" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="D55" s="16" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="19"/>
+        <v>70</v>
+      </c>
+      <c r="C56" s="15"/>
       <c r="D56" s="16" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
-        <v>14</v>
+      <c r="B57" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B58" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B58" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="20" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C63" s="11"/>
-      <c r="D63" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C64" s="21"/>
-      <c r="D64" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="21"/>
+      <c r="D63" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="12"/>
@@ -1433,119 +1439,123 @@
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-    </row>
-    <row r="70" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
+    <row r="69" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>10</v>
+      <c r="B71" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D72" s="3"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>29</v>
+    <row r="74" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D74" s="3"/>
     </row>
     <row r="75" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>9</v>
+      <c r="B77" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="15"/>
+      <c r="D77" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="19"/>
+      <c r="D79" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="15"/>
+      <c r="D80" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B80" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C81" s="15"/>
       <c r="D81" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B82" s="24" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="25"/>
       <c r="C82" s="15" t="s">
         <v>22</v>
       </c>
@@ -1553,132 +1563,132 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="25"/>
-      <c r="C83" s="15" t="s">
+    <row r="83" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="C83" s="21"/>
+      <c r="D83" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="2:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="21"/>
-      <c r="D84" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C90" s="23"/>
-      <c r="D90" s="23"/>
+    <row r="89" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>10</v>
+      <c r="B91" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="D91" s="3"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D92" s="3"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>29</v>
+    <row r="94" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D94" s="3"/>
     </row>
     <row r="95" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>9</v>
+      <c r="B97" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" s="15"/>
+      <c r="D97" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C98" s="15"/>
       <c r="D98" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B99" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="19"/>
+      <c r="D99" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B100" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" s="15"/>
+      <c r="D100" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B101" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="15"/>
-      <c r="D99" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B100" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C100" s="19"/>
-      <c r="D100" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B101" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C101" s="15"/>
       <c r="D101" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B102" s="24" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="25"/>
       <c r="C102" s="15" t="s">
         <v>22</v>
       </c>
@@ -1686,55 +1696,46 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="25"/>
-      <c r="C103" s="15" t="s">
-        <v>24</v>
-      </c>
+    <row r="103" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B103" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" s="15"/>
       <c r="D103" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B104" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C104" s="15"/>
-      <c r="D104" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B105" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C105" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D105" s="20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="27"/>
-      <c r="C106" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D106" s="17" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B104" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C104" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D104" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="27"/>
+      <c r="C105" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B48:B54"/>
-    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>